<commit_message>
Fixing bugs and systematizing dates
</commit_message>
<xml_diff>
--- a/Citizen_Kane_Continuity_Photos_2018_metadata.xlsx
+++ b/Citizen_Kane_Continuity_Photos_2018_metadata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam Sciolla\Documents\University_of_Michigan\2018_Winter\SI_675\Citizen_Kane_Continuity_Photographs_Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam Sciolla\Documents\University_of_Michigan\2018_Winter\SI_675\Citizen_Kane_Continuity_Photographs_Project\github_repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="208">
   <si>
     <t>Prints (#)</t>
   </si>
@@ -97,9 +97,6 @@
     <t>f1p2</t>
   </si>
   <si>
-    <t>Law Office Walter, Parks, and Thatcher</t>
-  </si>
-  <si>
     <t>f1p3</t>
   </si>
   <si>
@@ -142,21 +139,12 @@
     <t>TL: "2nd Floor - Enquirer Bldg - Prod. #281-15" TR: "Orson Welles"</t>
   </si>
   <si>
-    <t>TL: "RADIO PICTURES PRODUCTION #281 \n Citizen Kane"; BR: "SEP 25 '40 PM", clock time stamp showing 4:30</t>
-  </si>
-  <si>
     <t>f2p2</t>
   </si>
   <si>
-    <t>TL: "RADIO PICTURES PRODUCTION #281 \n Citizen Kane"; BR: "SEP 5 '40 PM", clock time stamp showing 5:50</t>
-  </si>
-  <si>
     <t>f2p4</t>
   </si>
   <si>
-    <t>TL: "RADIO PICTURES PRODUCTION #281 \n Citizen Kane"; BR: "SEP 10 '40 AM", clock time stamp showing 8:58</t>
-  </si>
-  <si>
     <t>f2p6</t>
   </si>
   <si>
@@ -166,9 +154,6 @@
     <t>f2p8</t>
   </si>
   <si>
-    <t>TL: "RADIO PICTURES PRODUCTION #281 \n Citizen Kane"; BR: "SEP 3 '40 AM", clock time stamp showing 8:35</t>
-  </si>
-  <si>
     <t>f2p9</t>
   </si>
   <si>
@@ -298,9 +283,6 @@
     <t>f4p7</t>
   </si>
   <si>
-    <t>Drug store, westside drug, street and lamp</t>
-  </si>
-  <si>
     <t>f4p8</t>
   </si>
   <si>
@@ -322,12 +304,6 @@
     <t>TL: "2nd Floor - Xanadu - Prod. #281-37"; TR: "Orson Welles"</t>
   </si>
   <si>
-    <t>TL: "RADIO PICTURES PRODUCTION #281 \n Citizen Kane"; BR: "OCT 23 '40 PM" and clock timestamp showing 2:48 p.m.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">xanadu ? --lavish room with equipment and decorations and no monkeys, vermin on ceiling </t>
-  </si>
-  <si>
     <t>f5p3</t>
   </si>
   <si>
@@ -490,9 +466,6 @@
     <t>f7p12</t>
   </si>
   <si>
-    <t>xanadu box frames statues, another staircase up to the right</t>
-  </si>
-  <si>
     <t>f7p13</t>
   </si>
   <si>
@@ -565,9 +538,6 @@
     <t>f9p7</t>
   </si>
   <si>
-    <t>chair xanadu dresser dolls, monkey</t>
-  </si>
-  <si>
     <t>f9p8</t>
   </si>
   <si>
@@ -695,6 +665,33 @@
   </si>
   <si>
     <t>TL: "RADIO PICTURES PRODUCTION #281 \n Citizen Kane"; BR: "OCT 15 '40 AM" and clock timestamp showing 10:28</t>
+  </si>
+  <si>
+    <t>TL: "RADIO PICTURES PRODUCTION #281 \n Citizen Kane"; BR: "OCT 23 '40 PM" and clock timestamp showing 2:48</t>
+  </si>
+  <si>
+    <t>Law Office Walter Parks and Thatcher</t>
+  </si>
+  <si>
+    <t>TL: "RADIO PICTURES PRODUCTION #281 \n Citizen Kane"; BR: "SEP 25 '40 PM"; clock time stamp showing 4:30</t>
+  </si>
+  <si>
+    <t>TL: "RADIO PICTURES PRODUCTION #281 \n Citizen Kane"; BR: "SEP 5 '40 PM"; clock time stamp showing 5:50</t>
+  </si>
+  <si>
+    <t>TL: "RADIO PICTURES PRODUCTION #281 \n Citizen Kane"; BR: "SEP 3 '40 AM"; clock time stamp showing 8:35</t>
+  </si>
+  <si>
+    <t>Drug store/westside drug/street and lamp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xanadu ? --lavish room with equipment and decorations and no monkeys/vermin on ceiling </t>
+  </si>
+  <si>
+    <t>xanadu box frames statues/another staircase up to the right</t>
+  </si>
+  <si>
+    <t>chair xanadu dresser dolls/monkey</t>
   </si>
 </sst>
 </file>
@@ -1636,6 +1633,114 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2809875</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="AutoShape 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F13880FE-239C-44E0-A1DD-37428234573A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="21097875" cy="8096250"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2809875</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="AutoShape 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91F0D2EE-F0C1-4EA6-9509-5BA5D2A81292}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="21097875" cy="8096250"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1938,9 +2043,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G58" sqref="G58"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H97" sqref="H97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1959,7 +2064,7 @@
   <sheetData>
     <row r="1" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="B1" s="17" t="s">
         <v>0</v>
@@ -1968,7 +2073,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="E1" s="17" t="s">
         <v>2</v>
@@ -1983,7 +2088,7 @@
         <v>5</v>
       </c>
       <c r="I1" s="33" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:24" s="5" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -2039,7 +2144,7 @@
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
       <c r="H3" s="16" t="s">
-        <v>9</v>
+        <v>200</v>
       </c>
       <c r="I3" s="15"/>
       <c r="J3" s="1"/>
@@ -2060,7 +2165,7 @@
     </row>
     <row r="4" spans="1:24" s="5" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="15">
         <v>0</v>
@@ -2075,7 +2180,7 @@
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
       <c r="H4" s="16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I4" s="15"/>
       <c r="J4" s="1"/>
@@ -2096,7 +2201,7 @@
     </row>
     <row r="5" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="17">
         <v>1</v>
@@ -2109,17 +2214,17 @@
         <v>3</v>
       </c>
       <c r="F5" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="17" t="s">
         <v>13</v>
-      </c>
-      <c r="G5" s="17" t="s">
-        <v>14</v>
       </c>
       <c r="H5" s="17"/>
       <c r="I5" s="33"/>
     </row>
     <row r="6" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="17">
         <v>1</v>
@@ -2132,17 +2237,17 @@
         <v>3</v>
       </c>
       <c r="F6" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="17" t="s">
         <v>13</v>
-      </c>
-      <c r="G6" s="17" t="s">
-        <v>14</v>
       </c>
       <c r="H6" s="17"/>
       <c r="I6" s="33"/>
     </row>
     <row r="7" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="17">
         <v>1</v>
@@ -2155,17 +2260,17 @@
         <v>3</v>
       </c>
       <c r="F7" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="17" t="s">
         <v>13</v>
-      </c>
-      <c r="G7" s="17" t="s">
-        <v>14</v>
       </c>
       <c r="H7" s="17"/>
       <c r="I7" s="33"/>
     </row>
     <row r="8" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="17">
         <v>1</v>
@@ -2178,17 +2283,17 @@
         <v>3</v>
       </c>
       <c r="F8" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="17" t="s">
         <v>13</v>
-      </c>
-      <c r="G8" s="17" t="s">
-        <v>14</v>
       </c>
       <c r="H8" s="17"/>
       <c r="I8" s="33"/>
     </row>
     <row r="9" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="17">
         <v>1</v>
@@ -2201,17 +2306,17 @@
         <v>3</v>
       </c>
       <c r="F9" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="17" t="s">
         <v>13</v>
-      </c>
-      <c r="G9" s="17" t="s">
-        <v>14</v>
       </c>
       <c r="H9" s="17"/>
       <c r="I9" s="33"/>
     </row>
     <row r="10" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" s="17">
         <v>1</v>
@@ -2224,17 +2329,17 @@
         <v>3</v>
       </c>
       <c r="F10" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="17" t="s">
         <v>13</v>
-      </c>
-      <c r="G10" s="17" t="s">
-        <v>14</v>
       </c>
       <c r="H10" s="17"/>
       <c r="I10" s="33"/>
     </row>
     <row r="11" spans="1:24" s="5" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" s="15">
         <v>0</v>
@@ -2249,7 +2354,7 @@
       <c r="F11" s="15"/>
       <c r="G11" s="15"/>
       <c r="H11" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I11" s="15"/>
       <c r="J11" s="1"/>
@@ -2270,7 +2375,7 @@
     </row>
     <row r="12" spans="1:24" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="46" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B12" s="46">
         <v>1</v>
@@ -2283,17 +2388,17 @@
         <v>2</v>
       </c>
       <c r="F12" s="46" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G12" s="46" t="s">
-        <v>24</v>
+        <v>201</v>
       </c>
       <c r="H12" s="46"/>
       <c r="I12" s="45"/>
     </row>
     <row r="13" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="17" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B13" s="17">
         <v>1</v>
@@ -2306,17 +2411,17 @@
         <v>3</v>
       </c>
       <c r="F13" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G13" s="17" t="s">
-        <v>26</v>
+        <v>202</v>
       </c>
       <c r="H13" s="17"/>
       <c r="I13" s="33"/>
     </row>
     <row r="14" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B14" s="17">
         <v>1</v>
@@ -2329,17 +2434,17 @@
         <v>3</v>
       </c>
       <c r="F14" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G14" s="17" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="H14" s="17"/>
       <c r="I14" s="33"/>
     </row>
     <row r="15" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B15" s="17">
         <v>1</v>
@@ -2352,17 +2457,17 @@
         <v>3</v>
       </c>
       <c r="F15" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G15" s="17" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H15" s="17"/>
       <c r="I15" s="33"/>
     </row>
     <row r="16" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B16" s="17">
         <v>1</v>
@@ -2375,17 +2480,17 @@
         <v>3</v>
       </c>
       <c r="F16" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>32</v>
+        <v>203</v>
       </c>
       <c r="H16" s="17"/>
       <c r="I16" s="33"/>
     </row>
     <row r="17" spans="1:24" s="10" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="18" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B17" s="19">
         <v>0</v>
@@ -2394,17 +2499,17 @@
         <v>1</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E17" s="19">
         <v>2</v>
       </c>
       <c r="F17" s="19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G17" s="19"/>
       <c r="H17" s="18" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="I17" s="19"/>
       <c r="J17" s="11"/>
@@ -2425,7 +2530,7 @@
     </row>
     <row r="18" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B18" s="17">
         <v>1</v>
@@ -2438,17 +2543,17 @@
         <v>3</v>
       </c>
       <c r="F18" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G18" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H18" s="17"/>
       <c r="I18" s="33"/>
     </row>
     <row r="19" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B19" s="17">
         <v>1</v>
@@ -2461,17 +2566,17 @@
         <v>3</v>
       </c>
       <c r="F19" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G19" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H19" s="17"/>
       <c r="I19" s="33"/>
     </row>
     <row r="20" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B20" s="17">
         <v>1</v>
@@ -2484,17 +2589,17 @@
         <v>3</v>
       </c>
       <c r="F20" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G20" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H20" s="17"/>
       <c r="I20" s="33"/>
     </row>
     <row r="21" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="17" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B21" s="17">
         <v>1</v>
@@ -2507,17 +2612,17 @@
         <v>3</v>
       </c>
       <c r="F21" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G21" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H21" s="17"/>
       <c r="I21" s="33"/>
     </row>
     <row r="22" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="17" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B22" s="17">
         <v>1</v>
@@ -2530,17 +2635,17 @@
         <v>3</v>
       </c>
       <c r="F22" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G22" s="17" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H22" s="17"/>
       <c r="I22" s="33"/>
     </row>
     <row r="23" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="17" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B23" s="17">
         <v>1</v>
@@ -2553,17 +2658,17 @@
         <v>3</v>
       </c>
       <c r="F23" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G23" s="17" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H23" s="17"/>
       <c r="I23" s="33"/>
     </row>
     <row r="24" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="17" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B24" s="17">
         <v>1</v>
@@ -2576,17 +2681,17 @@
         <v>3</v>
       </c>
       <c r="F24" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G24" s="17" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="H24" s="17"/>
       <c r="I24" s="33"/>
     </row>
     <row r="25" spans="1:24" s="5" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="15" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B25" s="15">
         <v>0</v>
@@ -2601,7 +2706,7 @@
       <c r="F25" s="15"/>
       <c r="G25" s="15"/>
       <c r="H25" s="16" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="I25" s="15"/>
       <c r="J25" s="1"/>
@@ -2622,7 +2727,7 @@
     </row>
     <row r="26" spans="1:24" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="36" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B26" s="36">
         <v>1</v>
@@ -2635,13 +2740,13 @@
         <v>3</v>
       </c>
       <c r="F26" s="36" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="G26" s="36" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H26" s="14" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="I26" s="36"/>
       <c r="J26" s="7"/>
@@ -2662,7 +2767,7 @@
     </row>
     <row r="27" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="17" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B27" s="17">
         <v>1</v>
@@ -2675,17 +2780,17 @@
         <v>3</v>
       </c>
       <c r="F27" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G27" s="17" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H27" s="17"/>
       <c r="I27" s="33"/>
     </row>
     <row r="28" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="17" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B28" s="17">
         <v>1</v>
@@ -2698,17 +2803,17 @@
         <v>3</v>
       </c>
       <c r="F28" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G28" s="17" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="H28" s="17"/>
       <c r="I28" s="33"/>
     </row>
     <row r="29" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="17" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B29" s="17">
         <v>1</v>
@@ -2721,17 +2826,17 @@
         <v>3</v>
       </c>
       <c r="F29" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G29" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H29" s="2"/>
       <c r="I29" s="33"/>
     </row>
     <row r="30" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="17" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B30" s="17">
         <v>1</v>
@@ -2744,17 +2849,17 @@
         <v>3</v>
       </c>
       <c r="F30" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G30" s="17" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="H30" s="17"/>
       <c r="I30" s="33"/>
     </row>
     <row r="31" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="17" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B31" s="17">
         <v>1</v>
@@ -2767,17 +2872,17 @@
         <v>3</v>
       </c>
       <c r="F31" s="17" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G31" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H31" s="17"/>
       <c r="I31" s="33"/>
     </row>
     <row r="32" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="17" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B32" s="17">
         <v>1</v>
@@ -2790,17 +2895,17 @@
         <v>3</v>
       </c>
       <c r="F32" s="17" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G32" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H32" s="17"/>
       <c r="I32" s="33"/>
     </row>
     <row r="33" spans="1:24" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="36" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B33" s="36">
         <v>1</v>
@@ -2813,19 +2918,19 @@
         <v>3</v>
       </c>
       <c r="F33" s="36" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G33" s="36" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H33" s="14" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="I33" s="37"/>
     </row>
     <row r="34" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="17" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B34" s="17">
         <v>1</v>
@@ -2838,17 +2943,17 @@
         <v>3</v>
       </c>
       <c r="F34" s="17" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G34" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H34" s="17"/>
       <c r="I34" s="33"/>
     </row>
     <row r="35" spans="1:24" s="41" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="36" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B35" s="36">
         <v>1</v>
@@ -2861,19 +2966,19 @@
         <v>3</v>
       </c>
       <c r="F35" s="14" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="G35" s="36" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H35" s="14" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="I35" s="14"/>
     </row>
     <row r="36" spans="1:24" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="46" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B36" s="46">
         <v>1</v>
@@ -2886,17 +2991,17 @@
         <v>2</v>
       </c>
       <c r="F36" s="46" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="G36" s="46" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="H36" s="46"/>
       <c r="I36" s="45"/>
     </row>
     <row r="37" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="17" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B37" s="17">
         <v>1</v>
@@ -2909,17 +3014,17 @@
         <v>3</v>
       </c>
       <c r="F37" s="17" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G37" s="17" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="H37" s="17"/>
       <c r="I37" s="33"/>
     </row>
     <row r="38" spans="1:24" s="5" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="20" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B38" s="20">
         <v>0</v>
@@ -2934,13 +3039,13 @@
       <c r="F38" s="20"/>
       <c r="G38" s="20"/>
       <c r="H38" s="13" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="I38" s="34"/>
     </row>
     <row r="39" spans="1:24" s="10" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="21" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B39" s="21">
         <v>0</v>
@@ -2949,13 +3054,13 @@
         <v>0</v>
       </c>
       <c r="D39" s="21" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="E39" s="21">
         <v>1</v>
       </c>
       <c r="F39" s="21" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="G39" s="21"/>
       <c r="H39" s="21"/>
@@ -2963,7 +3068,7 @@
     </row>
     <row r="40" spans="1:24" s="5" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="15" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B40" s="15">
         <v>0</v>
@@ -2978,7 +3083,7 @@
       <c r="F40" s="15"/>
       <c r="G40" s="15"/>
       <c r="H40" s="16" t="s">
-        <v>76</v>
+        <v>204</v>
       </c>
       <c r="I40" s="15"/>
       <c r="J40" s="1"/>
@@ -2999,7 +3104,7 @@
     </row>
     <row r="41" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="17" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B41" s="17">
         <v>1</v>
@@ -3012,17 +3117,17 @@
         <v>3</v>
       </c>
       <c r="F41" s="17" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="G41" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H41" s="17"/>
       <c r="I41" s="33"/>
     </row>
     <row r="42" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="17" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B42" s="17">
         <v>1</v>
@@ -3035,17 +3140,17 @@
         <v>3</v>
       </c>
       <c r="F42" s="17" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="G42" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H42" s="17"/>
       <c r="I42" s="33"/>
     </row>
     <row r="43" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="22" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B43" s="23">
         <v>1</v>
@@ -3058,17 +3163,17 @@
         <v>3</v>
       </c>
       <c r="F43" s="22" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="G43" s="22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H43" s="17"/>
       <c r="I43" s="33"/>
     </row>
     <row r="44" spans="1:24" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="39" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B44" s="40">
         <v>1</v>
@@ -3081,19 +3186,19 @@
         <v>3</v>
       </c>
       <c r="F44" s="39" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G44" s="39" t="s">
-        <v>84</v>
+        <v>199</v>
       </c>
       <c r="H44" s="14" t="s">
-        <v>85</v>
+        <v>205</v>
       </c>
       <c r="I44" s="37"/>
     </row>
     <row r="45" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="22" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="B45" s="23">
         <v>1</v>
@@ -3106,17 +3211,17 @@
         <v>3</v>
       </c>
       <c r="F45" s="22" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="G45" s="22" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H45" s="17"/>
       <c r="I45" s="33"/>
     </row>
     <row r="46" spans="1:24" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="42" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="B46" s="43">
         <v>1</v>
@@ -3129,19 +3234,19 @@
         <v>2</v>
       </c>
       <c r="F46" s="42" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="G46" s="42" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="H46" s="44" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="I46" s="45"/>
     </row>
     <row r="47" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="22" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B47" s="23">
         <v>1</v>
@@ -3154,17 +3259,17 @@
         <v>3</v>
       </c>
       <c r="F47" s="22" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="G47" s="22" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="H47" s="17"/>
       <c r="I47" s="33"/>
     </row>
     <row r="48" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="22" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="B48" s="23">
         <v>1</v>
@@ -3177,17 +3282,17 @@
         <v>3</v>
       </c>
       <c r="F48" s="22" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="G48" s="22" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="H48" s="17"/>
       <c r="I48" s="33"/>
     </row>
     <row r="49" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="22" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B49" s="23">
         <v>1</v>
@@ -3200,17 +3305,17 @@
         <v>3</v>
       </c>
       <c r="F49" s="22" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="G49" s="22" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="H49" s="17"/>
       <c r="I49" s="33"/>
     </row>
     <row r="50" spans="1:9" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="39" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B50" s="40">
         <v>1</v>
@@ -3223,19 +3328,19 @@
         <v>3</v>
       </c>
       <c r="F50" s="39" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G50" s="39" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="H50" s="14" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="I50" s="37"/>
     </row>
     <row r="51" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="22" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B51" s="23">
         <v>1</v>
@@ -3248,17 +3353,17 @@
         <v>3</v>
       </c>
       <c r="F51" s="22" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="G51" s="22" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="H51" s="17"/>
       <c r="I51" s="33"/>
     </row>
     <row r="52" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="22" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B52" s="23">
         <v>1</v>
@@ -3271,17 +3376,17 @@
         <v>3</v>
       </c>
       <c r="F52" s="22" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="G52" s="22" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="H52" s="17"/>
       <c r="I52" s="33"/>
     </row>
     <row r="53" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="22" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="B53" s="23">
         <v>1</v>
@@ -3294,17 +3399,17 @@
         <v>3</v>
       </c>
       <c r="F53" s="22" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="G53" s="22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H53" s="17"/>
       <c r="I53" s="33"/>
     </row>
     <row r="54" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="22" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="B54" s="23">
         <v>1</v>
@@ -3317,17 +3422,17 @@
         <v>3</v>
       </c>
       <c r="F54" s="22" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G54" s="22" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="H54" s="2"/>
       <c r="I54" s="33"/>
     </row>
     <row r="55" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="22" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="B55" s="23">
         <v>1</v>
@@ -3340,17 +3445,17 @@
         <v>3</v>
       </c>
       <c r="F55" s="22" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="G55" s="22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H55" s="2"/>
       <c r="I55" s="33"/>
     </row>
     <row r="56" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="17" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B56" s="17">
         <v>1</v>
@@ -3363,17 +3468,17 @@
         <v>3</v>
       </c>
       <c r="F56" s="17" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="G56" s="17" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="H56" s="17"/>
       <c r="I56" s="33"/>
     </row>
     <row r="57" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="17" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="B57" s="17">
         <v>1</v>
@@ -3386,17 +3491,17 @@
         <v>3</v>
       </c>
       <c r="F57" s="17" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="G57" s="17" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="H57" s="17"/>
       <c r="I57" s="33"/>
     </row>
     <row r="58" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="17" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="B58" s="17">
         <v>1</v>
@@ -3409,17 +3514,17 @@
         <v>3</v>
       </c>
       <c r="F58" s="17" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="G58" s="17" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="H58" s="17"/>
       <c r="I58" s="33"/>
     </row>
     <row r="59" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="17" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="B59" s="17">
         <v>1</v>
@@ -3432,17 +3537,17 @@
         <v>3</v>
       </c>
       <c r="F59" s="17" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="G59" s="17" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="H59" s="17"/>
       <c r="I59" s="33"/>
     </row>
     <row r="60" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="17" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="B60" s="17">
         <v>1</v>
@@ -3455,17 +3560,17 @@
         <v>3</v>
       </c>
       <c r="F60" s="17" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="G60" s="17" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="H60" s="17"/>
       <c r="I60" s="33"/>
     </row>
     <row r="61" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="17" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="B61" s="17">
         <v>1</v>
@@ -3478,17 +3583,17 @@
         <v>3</v>
       </c>
       <c r="F61" s="17" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="G61" s="17" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="H61" s="17"/>
       <c r="I61" s="33"/>
     </row>
     <row r="62" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" s="17" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="B62" s="17">
         <v>1</v>
@@ -3501,17 +3606,17 @@
         <v>3</v>
       </c>
       <c r="F62" s="17" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="G62" s="17" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="H62" s="17"/>
       <c r="I62" s="33"/>
     </row>
     <row r="63" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A63" s="17" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="B63" s="17">
         <v>1</v>
@@ -3524,17 +3629,17 @@
         <v>3</v>
       </c>
       <c r="F63" s="17" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="G63" s="17" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="H63" s="17"/>
       <c r="I63" s="33"/>
     </row>
     <row r="64" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A64" s="17" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="B64" s="17">
         <v>1</v>
@@ -3547,17 +3652,17 @@
         <v>3</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="H64" s="17"/>
       <c r="I64" s="33"/>
     </row>
     <row r="65" spans="1:24" s="5" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A65" s="24" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B65" s="24">
         <v>0</v>
@@ -3572,7 +3677,7 @@
       <c r="F65" s="24"/>
       <c r="G65" s="24"/>
       <c r="H65" s="26" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="I65" s="24"/>
       <c r="J65" s="9"/>
@@ -3593,7 +3698,7 @@
     </row>
     <row r="66" spans="1:24" s="5" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A66" s="24" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="B66" s="24">
         <v>0</v>
@@ -3608,7 +3713,7 @@
       <c r="F66" s="24"/>
       <c r="G66" s="24"/>
       <c r="H66" s="26" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="I66" s="24"/>
       <c r="J66" s="9"/>
@@ -3629,7 +3734,7 @@
     </row>
     <row r="67" spans="1:24" s="5" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A67" s="24" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B67" s="24">
         <v>0</v>
@@ -3644,7 +3749,7 @@
       <c r="F67" s="24"/>
       <c r="G67" s="24"/>
       <c r="H67" s="26" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="I67" s="24"/>
       <c r="J67" s="9"/>
@@ -3665,7 +3770,7 @@
     </row>
     <row r="68" spans="1:24" s="10" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A68" s="21" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B68" s="21">
         <v>0</v>
@@ -3674,13 +3779,13 @@
         <v>0</v>
       </c>
       <c r="D68" s="21" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="E68" s="21">
         <v>1</v>
       </c>
       <c r="F68" s="27" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="G68" s="21"/>
       <c r="H68" s="28"/>
@@ -3688,7 +3793,7 @@
     </row>
     <row r="69" spans="1:24" s="5" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A69" s="24" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="B69" s="24">
         <v>0</v>
@@ -3703,7 +3808,7 @@
       <c r="F69" s="24"/>
       <c r="G69" s="24"/>
       <c r="H69" s="26" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="I69" s="24"/>
       <c r="J69" s="9"/>
@@ -3724,7 +3829,7 @@
     </row>
     <row r="70" spans="1:24" s="10" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A70" s="21" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="B70" s="21">
         <v>0</v>
@@ -3733,13 +3838,13 @@
         <v>0</v>
       </c>
       <c r="D70" s="21" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="E70" s="21">
         <v>1</v>
       </c>
       <c r="F70" s="27" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="G70" s="21"/>
       <c r="H70" s="28"/>
@@ -3747,7 +3852,7 @@
     </row>
     <row r="71" spans="1:24" s="5" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A71" s="24" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="B71" s="24">
         <v>0</v>
@@ -3762,7 +3867,7 @@
       <c r="F71" s="24"/>
       <c r="G71" s="24"/>
       <c r="H71" s="26" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="I71" s="24"/>
       <c r="J71" s="9"/>
@@ -3783,7 +3888,7 @@
     </row>
     <row r="72" spans="1:24" s="10" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A72" s="21" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="B72" s="21">
         <v>0</v>
@@ -3792,13 +3897,13 @@
         <v>0</v>
       </c>
       <c r="D72" s="21" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="E72" s="21">
         <v>1</v>
       </c>
       <c r="F72" s="27" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="G72" s="21"/>
       <c r="H72" s="28"/>
@@ -3806,7 +3911,7 @@
     </row>
     <row r="73" spans="1:24" s="5" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A73" s="24" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="B73" s="24">
         <v>0</v>
@@ -3821,7 +3926,7 @@
       <c r="F73" s="24"/>
       <c r="G73" s="24"/>
       <c r="H73" s="26" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="I73" s="24"/>
       <c r="J73" s="9"/>
@@ -3842,7 +3947,7 @@
     </row>
     <row r="74" spans="1:24" s="5" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A74" s="24" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="B74" s="24">
         <v>0</v>
@@ -3857,7 +3962,7 @@
       <c r="F74" s="24"/>
       <c r="G74" s="24"/>
       <c r="H74" s="26" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="I74" s="24"/>
       <c r="J74" s="9"/>
@@ -3878,7 +3983,7 @@
     </row>
     <row r="75" spans="1:24" s="5" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A75" s="24" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="B75" s="24">
         <v>0</v>
@@ -3893,7 +3998,7 @@
       <c r="F75" s="24"/>
       <c r="G75" s="24"/>
       <c r="H75" s="26" t="s">
-        <v>140</v>
+        <v>206</v>
       </c>
       <c r="I75" s="24"/>
       <c r="J75" s="9"/>
@@ -3914,7 +4019,7 @@
     </row>
     <row r="76" spans="1:24" s="10" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A76" s="21" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="B76" s="21">
         <v>0</v>
@@ -3923,13 +4028,13 @@
         <v>0</v>
       </c>
       <c r="D76" s="21" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="E76" s="21">
         <v>1</v>
       </c>
       <c r="F76" s="27" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="G76" s="21"/>
       <c r="H76" s="28"/>
@@ -3937,7 +4042,7 @@
     </row>
     <row r="77" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A77" s="17" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="B77" s="17">
         <v>1</v>
@@ -3950,17 +4055,17 @@
         <v>3</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="G77" s="2" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="H77" s="17"/>
       <c r="I77" s="33"/>
     </row>
     <row r="78" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A78" s="17" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="B78" s="17">
         <v>1</v>
@@ -3973,17 +4078,17 @@
         <v>3</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="G78" s="2" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="H78" s="2"/>
       <c r="I78" s="33"/>
     </row>
     <row r="79" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A79" s="17" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="B79" s="17">
         <v>1</v>
@@ -3996,17 +4101,17 @@
         <v>3</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="G79" s="2" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="H79" s="17"/>
       <c r="I79" s="33"/>
     </row>
     <row r="80" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A80" s="17" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="B80" s="17">
         <v>1</v>
@@ -4019,17 +4124,17 @@
         <v>3</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="G80" s="2" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="H80" s="17"/>
       <c r="I80" s="33"/>
     </row>
     <row r="81" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A81" s="17" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="B81" s="17">
         <v>1</v>
@@ -4042,17 +4147,17 @@
         <v>3</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="G81" s="2" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="H81" s="17"/>
       <c r="I81" s="33"/>
     </row>
     <row r="82" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A82" s="17" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="B82" s="17">
         <v>1</v>
@@ -4065,17 +4170,17 @@
         <v>3</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="G82" s="29" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="H82" s="17"/>
       <c r="I82" s="33"/>
     </row>
     <row r="83" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A83" s="17" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="B83" s="17">
         <v>1</v>
@@ -4088,17 +4193,17 @@
         <v>3</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="G83" s="29" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="H83" s="17"/>
       <c r="I83" s="33"/>
     </row>
     <row r="84" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A84" s="17" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="B84" s="17">
         <v>1</v>
@@ -4111,17 +4216,17 @@
         <v>3</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="G84" s="29" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="H84" s="17"/>
       <c r="I84" s="33"/>
     </row>
     <row r="85" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A85" s="17" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B85" s="17">
         <v>1</v>
@@ -4134,17 +4239,17 @@
         <v>3</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="G85" s="29" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="H85" s="17"/>
       <c r="I85" s="33"/>
     </row>
     <row r="86" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A86" s="17" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="B86" s="17">
         <v>1</v>
@@ -4157,17 +4262,17 @@
         <v>3</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="G86" s="29" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="H86" s="17"/>
       <c r="I86" s="33"/>
     </row>
     <row r="87" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A87" s="17" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="B87" s="17">
         <v>1</v>
@@ -4180,17 +4285,17 @@
         <v>3</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="G87" s="17" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="H87" s="17"/>
       <c r="I87" s="33"/>
     </row>
     <row r="88" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A88" s="17" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="B88" s="17">
         <v>1</v>
@@ -4203,17 +4308,17 @@
         <v>3</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="G88" s="12" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="H88" s="17"/>
       <c r="I88" s="33"/>
     </row>
     <row r="89" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A89" s="17" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="B89" s="17">
         <v>1</v>
@@ -4226,17 +4331,17 @@
         <v>3</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="G89" s="2" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="H89" s="17"/>
       <c r="I89" s="33"/>
     </row>
     <row r="90" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A90" s="17" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="B90" s="17">
         <v>1</v>
@@ -4249,17 +4354,17 @@
         <v>3</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="G90" s="29" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="H90" s="17"/>
       <c r="I90" s="33"/>
     </row>
     <row r="91" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A91" s="30" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="B91" s="30">
         <v>1</v>
@@ -4272,10 +4377,10 @@
         <v>3</v>
       </c>
       <c r="F91" s="31" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="G91" s="29" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="H91" s="30"/>
       <c r="I91" s="30"/>
@@ -4297,7 +4402,7 @@
     </row>
     <row r="92" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A92" s="17" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="B92" s="17">
         <v>1</v>
@@ -4310,17 +4415,17 @@
         <v>3</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="G92" s="2" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="H92" s="17"/>
       <c r="I92" s="33"/>
     </row>
     <row r="93" spans="1:24" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A93" s="36" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="B93" s="36">
         <v>1</v>
@@ -4333,19 +4438,19 @@
         <v>3</v>
       </c>
       <c r="F93" s="14" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="G93" s="14" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="H93" s="14" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="I93" s="37"/>
     </row>
     <row r="94" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A94" s="17" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="B94" s="17">
         <v>1</v>
@@ -4358,17 +4463,17 @@
         <v>3</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="G94" s="2" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="H94" s="17"/>
       <c r="I94" s="33"/>
     </row>
     <row r="95" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="30" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="B95" s="30">
         <v>1</v>
@@ -4381,10 +4486,10 @@
         <v>3</v>
       </c>
       <c r="F95" s="31" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="G95" s="29" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="H95" s="30"/>
       <c r="I95" s="30"/>
@@ -4406,7 +4511,7 @@
     </row>
     <row r="96" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A96" s="17" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="B96" s="17">
         <v>1</v>
@@ -4419,19 +4524,19 @@
         <v>3</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="G96" s="2" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="H96" s="2" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="I96" s="33"/>
     </row>
     <row r="97" spans="1:24" s="5" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A97" s="24" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="B97" s="24">
         <v>0</v>
@@ -4446,7 +4551,7 @@
       <c r="F97" s="24"/>
       <c r="G97" s="24"/>
       <c r="H97" s="25" t="s">
-        <v>165</v>
+        <v>207</v>
       </c>
       <c r="I97" s="24"/>
       <c r="J97" s="9"/>
@@ -4467,7 +4572,7 @@
     </row>
     <row r="98" spans="1:24" s="10" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A98" s="21" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B98" s="21">
         <v>0</v>
@@ -4476,13 +4581,13 @@
         <v>0</v>
       </c>
       <c r="D98" s="21" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="E98" s="21">
         <v>1</v>
       </c>
       <c r="F98" s="27" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="G98" s="21"/>
       <c r="H98" s="21"/>
@@ -4490,7 +4595,7 @@
     </row>
     <row r="99" spans="1:24" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A99" s="36" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="B99" s="36">
         <v>1</v>
@@ -4503,19 +4608,19 @@
         <v>3</v>
       </c>
       <c r="F99" s="14" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="G99" s="14" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="H99" s="14" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="I99" s="37"/>
     </row>
     <row r="100" spans="1:24" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A100" s="36" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="B100" s="36">
         <v>1</v>
@@ -4528,19 +4633,19 @@
         <v>3</v>
       </c>
       <c r="F100" s="14" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="G100" s="38" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="H100" s="14" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="I100" s="37"/>
     </row>
     <row r="101" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A101" s="17" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="B101" s="17">
         <v>1</v>
@@ -4553,17 +4658,17 @@
         <v>3</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="G101" s="2" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="H101" s="33"/>
       <c r="I101" s="33"/>
     </row>
     <row r="102" spans="1:24" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A102" s="36" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="B102" s="36">
         <v>1</v>
@@ -4576,13 +4681,13 @@
         <v>3</v>
       </c>
       <c r="F102" s="14" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="G102" s="14" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="H102" s="14" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="I102" s="36"/>
       <c r="J102" s="7"/>
@@ -4603,7 +4708,7 @@
     </row>
     <row r="103" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A103" s="17" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="B103" s="17">
         <v>1</v>
@@ -4616,19 +4721,19 @@
         <v>3</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="G103" s="32" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="H103" s="2" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="I103" s="33"/>
     </row>
     <row r="104" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A104" s="17" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="B104" s="17">
         <v>1</v>
@@ -4641,17 +4746,17 @@
         <v>3</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="G104" s="29" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="H104" s="33"/>
       <c r="I104" s="33"/>
     </row>
     <row r="105" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A105" s="17" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="B105" s="17">
         <v>1</v>
@@ -4664,10 +4769,10 @@
         <v>3</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="G105" s="29" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="H105" s="33"/>
       <c r="I105" s="33"/>

</xml_diff>